<commit_message>
Fixing and updating to new digisales mobile
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/DigisalesLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/DigisalesLib_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A942E12-E340-4801-BE5F-7A019D8FFE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53941869-8204-45BD-B337-E1CEF9BB9602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>Automation Tester 2</t>
   </si>
   <si>
-    <t>http://192.168.231.13:85/</t>
-  </si>
-  <si>
     <t>URL_DIGISALESMOBILE</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>filezilla</t>
+  </si>
+  <si>
+    <t>http://192.168.231.13:99/</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
         <v>22</v>
@@ -644,22 +644,22 @@
         <v>15</v>
       </c>
       <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>44</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>23</v>
@@ -712,16 +712,16 @@
         <v>35</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="AA2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun SCD0338-017 and Fixing SCD0338-008
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/DigisalesLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/DigisalesLib_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53941869-8204-45BD-B337-E1CEF9BB9602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E11C79-7877-4C95-9AD1-1099B7B94CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>